<commit_message>
Fixed basic_7 input; Added discontinuity check when negotiationg to avoid breaking up splits
</commit_message>
<xml_diff>
--- a/result-highlighted.xlsx
+++ b/result-highlighted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codee\package_splitter\splitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{50ED6B43-9FE7-46ED-A43C-2A57A3E497C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EE7D55-C752-4233-80BF-176681853041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -545,77 +545,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -988,11 +918,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,28 +935,28 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1037,380 +967,1213 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J11">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J12">
-        <v>7</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Upgraded to read 4 colour input graph
</commit_message>
<xml_diff>
--- a/result-highlighted.xlsx
+++ b/result-highlighted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codee\package_splitter\splitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731545D5-9120-4EE0-BA17-0D3A5C437C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4589DC95-FA07-4D11-9D0B-955833E9ED83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,7 +560,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="54">
     <dxf>
       <fill>
         <patternFill>
@@ -606,77 +606,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor rgb="FFCB7FB5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -760,6 +690,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFBE7CB0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -802,7 +739,63 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor rgb="FFCB7FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -948,6 +941,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFBE7CB0"/>
+      <color rgb="FFCB7FB5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1258,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="AT43" sqref="AT43"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="V188" sqref="V188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18286,13 +18285,13 @@
         <v>1</v>
       </c>
       <c r="N169" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O169" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P169" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q169" s="1">
         <v>2</v>
@@ -18328,40 +18327,40 @@
         <v>2</v>
       </c>
       <c r="AB169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM169" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -18387,13 +18386,13 @@
         <v>2</v>
       </c>
       <c r="S170" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T170" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U170" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V170" s="1">
         <v>2</v>
@@ -18405,81 +18404,81 @@
         <v>2</v>
       </c>
       <c r="Y170" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z170" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA170" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB170" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC170" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD170" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE170" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF170" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG170" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH170" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI170" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ170" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK170" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL170" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM170" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L171" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M171" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N171" s="1">
         <v>1</v>
       </c>
       <c r="O171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U171" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V171" s="1">
         <v>2</v>
@@ -18491,81 +18490,81 @@
         <v>2</v>
       </c>
       <c r="Y171" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z171" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA171" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB171" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC171" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD171" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE171" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF171" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG171" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH171" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI171" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ171" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK171" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL171" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM171" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L172" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M172" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N172" s="1">
         <v>1</v>
       </c>
       <c r="O172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U172" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V172" s="1">
         <v>2</v>
@@ -18577,81 +18576,81 @@
         <v>2</v>
       </c>
       <c r="Y172" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z172" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA172" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB172" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC172" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD172" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE172" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF172" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG172" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH172" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI172" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ172" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK172" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL172" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM172" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L173" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M173" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N173" s="1">
         <v>1</v>
       </c>
       <c r="O173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U173" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V173" s="1">
         <v>2</v>
@@ -18663,229 +18662,229 @@
         <v>2</v>
       </c>
       <c r="Y173" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z173" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA173" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB173" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC173" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD173" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE173" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF173" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG173" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH173" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI173" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ173" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK173" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL173" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM173" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L174" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M174" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N174" s="1">
         <v>1</v>
       </c>
       <c r="O174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U174" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V174" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W174" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X174" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y174" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z174" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH174" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI174" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ174" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AK174" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AL174" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM174" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L175" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M175" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N175" s="1">
         <v>1</v>
       </c>
       <c r="O175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U175" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V175" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W175" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X175" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y175" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z175" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH175" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI175" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ175" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AK175" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AL175" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM175" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L176" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M176" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N176" s="1">
         <v>1</v>
@@ -18912,66 +18911,66 @@
         <v>1</v>
       </c>
       <c r="V176" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W176" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X176" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y176" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z176" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH176" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI176" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ176" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AK176" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AL176" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM176" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L177" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M177" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N177" s="1">
         <v>1</v>
@@ -18983,10 +18982,10 @@
         <v>1</v>
       </c>
       <c r="Q177" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R177" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S177" s="1">
         <v>1</v>
@@ -19004,60 +19003,60 @@
         <v>1</v>
       </c>
       <c r="X177" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y177" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z177" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH177" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI177" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ177" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AK177" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AL177" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM177" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L178" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M178" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N178" s="1">
         <v>1</v>
@@ -19069,10 +19068,10 @@
         <v>1</v>
       </c>
       <c r="Q178" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R178" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S178" s="1">
         <v>1</v>
@@ -19090,60 +19089,60 @@
         <v>1</v>
       </c>
       <c r="X178" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y178" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z178" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH178" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI178" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ178" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AK178" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AL178" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM178" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L179" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M179" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N179" s="1">
         <v>1</v>
@@ -19155,10 +19154,10 @@
         <v>1</v>
       </c>
       <c r="Q179" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R179" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S179" s="1">
         <v>1</v>
@@ -19176,60 +19175,60 @@
         <v>1</v>
       </c>
       <c r="X179" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Y179" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z179" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AA179" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB179" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC179" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD179" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE179" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF179" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG179" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH179" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI179" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ179" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AK179" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AL179" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM179" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L180" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M180" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N180" s="1">
         <v>1</v>
@@ -19241,10 +19240,10 @@
         <v>1</v>
       </c>
       <c r="Q180" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R180" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S180" s="1">
         <v>6</v>
@@ -19262,25 +19261,25 @@
         <v>6</v>
       </c>
       <c r="X180" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Y180" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z180" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AA180" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB180" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC180" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD180" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE180" s="1">
         <v>5</v>
@@ -19304,18 +19303,18 @@
         <v>5</v>
       </c>
       <c r="AL180" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM180" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L181" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M181" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N181" s="1">
         <v>1</v>
@@ -19348,25 +19347,25 @@
         <v>6</v>
       </c>
       <c r="X181" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Y181" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z181" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AA181" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB181" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC181" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD181" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE181" s="1">
         <v>5</v>
@@ -19390,18 +19389,18 @@
         <v>5</v>
       </c>
       <c r="AL181" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AM181" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="182" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L182" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M182" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N182" s="1">
         <v>1</v>
@@ -19434,81 +19433,81 @@
         <v>6</v>
       </c>
       <c r="X182" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Y182" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z182" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AA182" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB182" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC182" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD182" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AH182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM182" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="183" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L183" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M183" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N183" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O183" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P183" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q183" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R183" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S183" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="T183" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="U183" s="1">
         <v>6</v>
@@ -19520,155 +19519,155 @@
         <v>6</v>
       </c>
       <c r="X183" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y183" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z183" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA183" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB183" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC183" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD183" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AH183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM183" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="184" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L184" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M184" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N184" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O184" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P184" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q184" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R184" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S184" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="T184" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="U184" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="V184" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="W184" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="X184" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y184" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z184" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA184" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB184" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC184" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD184" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AF184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AH184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM184" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="185" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L185" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M185" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N185" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O185" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P185" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q185" s="1">
         <v>9</v>
@@ -19677,84 +19676,84 @@
         <v>9</v>
       </c>
       <c r="S185" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="T185" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="U185" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="V185" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="W185" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="X185" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y185" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z185" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA185" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB185" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC185" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD185" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE185" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF185" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG185" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH185" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI185" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ185" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK185" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL185" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM185" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="186" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L186" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M186" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N186" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O186" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P186" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q186" s="1">
         <v>9</v>
@@ -19763,10 +19762,10 @@
         <v>9</v>
       </c>
       <c r="S186" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="T186" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="U186" s="1">
         <v>9</v>
@@ -19778,69 +19777,69 @@
         <v>9</v>
       </c>
       <c r="X186" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y186" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z186" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA186" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB186" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC186" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD186" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE186" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF186" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG186" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH186" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI186" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ186" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK186" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL186" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM186" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L187" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M187" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N187" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O187" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P187" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q187" s="1">
         <v>9</v>
@@ -19870,63 +19869,63 @@
         <v>9</v>
       </c>
       <c r="Z187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AA187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG187" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH187" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI187" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ187" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK187" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL187" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM187" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="188" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L188" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M188" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N188" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O188" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P188" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q188" s="1">
         <v>9</v>
@@ -19956,63 +19955,63 @@
         <v>9</v>
       </c>
       <c r="Z188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AA188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG188" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH188" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI188" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ188" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK188" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL188" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM188" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="189" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L189" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M189" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N189" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O189" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P189" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q189" s="1">
         <v>9</v>
@@ -20042,51 +20041,51 @@
         <v>9</v>
       </c>
       <c r="Z189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AA189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI189" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AJ189" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK189" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL189" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM189" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="190" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L190" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M190" s="1">
         <v>9</v>
@@ -20128,51 +20127,51 @@
         <v>9</v>
       </c>
       <c r="Z190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AA190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI190" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AJ190" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK190" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL190" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM190" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="191" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L191" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M191" s="1">
         <v>9</v>
@@ -20187,73 +20186,73 @@
         <v>9</v>
       </c>
       <c r="Q191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Y191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AA191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI191" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AJ191" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK191" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL191" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM191" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="192" spans="12:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20337,13 +20336,13 @@
     <row r="270" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">

</xml_diff>